<commit_message>
fixed refund request end point and added some comments to the to-do (Please Check)
</commit_message>
<xml_diff>
--- a/Our SE ms2&3 evaluation.xlsx
+++ b/Our SE ms2&3 evaluation.xlsx
@@ -6533,10 +6533,10 @@
   <dimension ref="A1:D1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C77" sqref="C77"/>
+      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -7406,11 +7406,11 @@
       </c>
       <c r="B77" s="86"/>
       <c r="C77" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77" s="81">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" customHeight="1">
@@ -7468,7 +7468,7 @@
       <c r="C82" s="13"/>
       <c r="D82" s="90">
         <f>SUM(D76:D80)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15.75" customHeight="1">
@@ -7744,7 +7744,7 @@
       <c r="C107" s="31"/>
       <c r="D107" s="95">
         <f>SUM(D28,D35,D49,D67,D82,D86,D93,D105)</f>
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15.75" customHeight="1">
@@ -9134,7 +9134,7 @@
       <c r="B234" s="77"/>
       <c r="C234" s="61">
         <f>SUM(D221,D107)</f>
-        <v>407.5</v>
+        <v>412.5</v>
       </c>
       <c r="D234" s="76"/>
     </row>
@@ -9168,7 +9168,7 @@
       <c r="B238" s="77"/>
       <c r="C238" s="37">
         <f>SUM(D221,D107)</f>
-        <v>407.5</v>
+        <v>412.5</v>
       </c>
       <c r="D238" s="76"/>
     </row>
@@ -9190,7 +9190,7 @@
       <c r="B241" s="77"/>
       <c r="C241" s="37">
         <f>SUM(C238,5)</f>
-        <v>412.5</v>
+        <v>417.5</v>
       </c>
       <c r="D241" s="76"/>
     </row>
@@ -9282,7 +9282,7 @@
       <c r="B254" s="77"/>
       <c r="C254" s="37">
         <f>SUM(C241:C252)</f>
-        <v>422.5</v>
+        <v>427.5</v>
       </c>
       <c r="D254" s="76"/>
     </row>

</xml_diff>